<commit_message>
Updating CDW input data
</commit_message>
<xml_diff>
--- a/cdw_tallyAnalysis/D17/D17-SOAP-2023_cdw_tally_prod_child.xlsx
+++ b/cdw_tallyAnalysis/D17/D17-SOAP-2023_cdw_tally_prod_child.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmeier/Documents/gitRepositories/neon-plant-sampling/cdw_tallyAnalysis/D17/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5738923A-7863-5645-9E95-FE8B708A12A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB313883-C701-0944-AD11-3D19D543750C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="37340" windowHeight="28300" xr2:uid="{75547C8C-A164-894F-9105-1D1F1743C90B}"/>
+    <workbookView xWindow="12500" yWindow="500" windowWidth="37340" windowHeight="28300" xr2:uid="{75547C8C-A164-894F-9105-1D1F1743C90B}"/>
   </bookViews>
   <sheets>
     <sheet name="cdw_tally_prod_cdw_transect" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11811" uniqueCount="3276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11835" uniqueCount="3281">
   <si>
     <t>_child_record_id</t>
   </si>
@@ -9849,13 +9849,28 @@
   </si>
   <si>
     <t>charextent</t>
+  </si>
+  <si>
+    <t>25-50</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>95-100</t>
+  </si>
+  <si>
+    <t>5-25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -9970,6 +9985,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos"/>
       <family val="2"/>
     </font>
@@ -10315,13 +10336,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10700,8 +10723,8 @@
   <dimension ref="A1:DH274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CP1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="DG2" sqref="DG2"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="DG54" sqref="DG54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10713,6 +10736,8 @@
     <col min="95" max="95" width="23.5" customWidth="1"/>
     <col min="96" max="102" width="0" hidden="1" customWidth="1"/>
     <col min="103" max="103" width="55.83203125" style="2" customWidth="1"/>
+    <col min="110" max="110" width="17" bestFit="1" customWidth="1"/>
+    <col min="111" max="112" width="15.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:112" ht="17" x14ac:dyDescent="0.2">
@@ -11046,10 +11071,10 @@
       <c r="DF1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DG1" s="4" t="s">
         <v>3275</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DH1" s="4" t="s">
         <v>3274</v>
       </c>
     </row>
@@ -11231,6 +11256,12 @@
       <c r="DE2" t="s">
         <v>143</v>
       </c>
+      <c r="DG2" s="4" t="s">
+        <v>3276</v>
+      </c>
+      <c r="DH2" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
     <row r="3" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -16569,7 +16600,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>504</v>
       </c>
@@ -16748,7 +16779,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>520</v>
       </c>
@@ -16926,8 +16957,14 @@
       <c r="DE34" t="s">
         <v>143</v>
       </c>
+      <c r="DG34" s="4" t="s">
+        <v>3277</v>
+      </c>
+      <c r="DH34" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="35" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>532</v>
       </c>
@@ -17109,7 +17146,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>543</v>
       </c>
@@ -17285,7 +17322,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>554</v>
       </c>
@@ -17461,7 +17498,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>564</v>
       </c>
@@ -17637,7 +17674,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>576</v>
       </c>
@@ -17816,7 +17853,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>588</v>
       </c>
@@ -17994,8 +18031,14 @@
       <c r="DE40" t="s">
         <v>143</v>
       </c>
+      <c r="DG40" s="4" t="s">
+        <v>3277</v>
+      </c>
+      <c r="DH40" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="41" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>603</v>
       </c>
@@ -18173,8 +18216,14 @@
       <c r="DE41" t="s">
         <v>143</v>
       </c>
+      <c r="DG41" s="4" t="s">
+        <v>3277</v>
+      </c>
+      <c r="DH41" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="42" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>614</v>
       </c>
@@ -18355,8 +18404,14 @@
       <c r="DE42" t="s">
         <v>143</v>
       </c>
+      <c r="DG42" s="4" t="s">
+        <v>3276</v>
+      </c>
+      <c r="DH42" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="43" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>626</v>
       </c>
@@ -18534,8 +18589,14 @@
       <c r="DE43" t="s">
         <v>143</v>
       </c>
+      <c r="DG43" s="4" t="s">
+        <v>3279</v>
+      </c>
+      <c r="DH43" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="44" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>638</v>
       </c>
@@ -18716,8 +18777,14 @@
       <c r="DE44" t="s">
         <v>143</v>
       </c>
+      <c r="DG44" s="4" t="s">
+        <v>3277</v>
+      </c>
+      <c r="DH44" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="45" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>650</v>
       </c>
@@ -18898,8 +18965,14 @@
       <c r="DE45" t="s">
         <v>143</v>
       </c>
+      <c r="DG45" s="4" t="s">
+        <v>3280</v>
+      </c>
+      <c r="DH45" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="46" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>662</v>
       </c>
@@ -19078,7 +19151,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>673</v>
       </c>
@@ -19257,7 +19330,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>683</v>
       </c>
@@ -19436,7 +19509,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:109" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:112" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>695</v>
       </c>
@@ -19614,8 +19687,14 @@
       <c r="DE49" t="s">
         <v>143</v>
       </c>
+      <c r="DG49" s="4" t="s">
+        <v>3277</v>
+      </c>
+      <c r="DH49" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="50" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>706</v>
       </c>
@@ -19794,7 +19873,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>718</v>
       </c>
@@ -19978,8 +20057,14 @@
       <c r="DE51" t="s">
         <v>143</v>
       </c>
+      <c r="DG51" s="4" t="s">
+        <v>3280</v>
+      </c>
+      <c r="DH51" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="52" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>731</v>
       </c>
@@ -20157,8 +20242,14 @@
       <c r="DE52" t="s">
         <v>143</v>
       </c>
+      <c r="DG52" s="4" t="s">
+        <v>3277</v>
+      </c>
+      <c r="DH52" s="4" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="53" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>746</v>
       </c>
@@ -20336,8 +20427,14 @@
       <c r="DE53" t="s">
         <v>143</v>
       </c>
+      <c r="DG53" s="4" t="s">
+        <v>3276</v>
+      </c>
+      <c r="DH53" s="5" t="s">
+        <v>3278</v>
+      </c>
     </row>
-    <row r="54" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>758</v>
       </c>
@@ -20516,7 +20613,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>769</v>
       </c>
@@ -20695,7 +20792,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>780</v>
       </c>
@@ -20880,7 +20977,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>795</v>
       </c>
@@ -21059,7 +21156,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>808</v>
       </c>
@@ -21241,7 +21338,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>820</v>
       </c>
@@ -21423,7 +21520,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>832</v>
       </c>
@@ -21602,7 +21699,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>843</v>
       </c>
@@ -21784,7 +21881,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:109" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>855</v>
       </c>
@@ -21963,7 +22060,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="63" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>868</v>
       </c>
@@ -22142,7 +22239,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>884</v>
       </c>
@@ -59583,5 +59680,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding chardepth and charextent LOV
</commit_message>
<xml_diff>
--- a/cdw_tallyAnalysis/D17/D17-SOAP-2023_cdw_tally_prod_child.xlsx
+++ b/cdw_tallyAnalysis/D17/D17-SOAP-2023_cdw_tally_prod_child.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmeier/Documents/gitRepositories/neon-plant-sampling/cdw_tallyAnalysis/D17/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB313883-C701-0944-AD11-3D19D543750C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2168AD-1D66-4344-994D-FEDDDEEF2CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12500" yWindow="500" windowWidth="37340" windowHeight="28300" xr2:uid="{75547C8C-A164-894F-9105-1D1F1743C90B}"/>
+    <workbookView xWindow="12500" yWindow="500" windowWidth="37340" windowHeight="28300" activeTab="1" xr2:uid="{75547C8C-A164-894F-9105-1D1F1743C90B}"/>
   </bookViews>
   <sheets>
     <sheet name="cdw_tally_prod_cdw_transect" sheetId="1" r:id="rId1"/>
+    <sheet name="LOV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11835" uniqueCount="3281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11929" uniqueCount="3288">
   <si>
     <t>_child_record_id</t>
   </si>
@@ -9854,9 +9855,6 @@
     <t>25-50</t>
   </si>
   <si>
-    <t>0-5</t>
-  </si>
-  <si>
     <t>0-1</t>
   </si>
   <si>
@@ -9864,6 +9862,30 @@
   </si>
   <si>
     <t>5-25</t>
+  </si>
+  <si>
+    <t>&gt; 1</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>6-25</t>
+  </si>
+  <si>
+    <t>26-50</t>
+  </si>
+  <si>
+    <t>51-75</t>
+  </si>
+  <si>
+    <t>76-95</t>
+  </si>
+  <si>
+    <t>96-100</t>
   </si>
 </sst>
 </file>
@@ -10722,9 +10744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F909FCEB-79A7-4B42-8C26-5A6A123C8280}">
   <dimension ref="A1:DH274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CP1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="DG54" sqref="DG54"/>
+    <sheetView topLeftCell="CP1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="DF49" sqref="DF49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11260,7 +11282,7 @@
         <v>3276</v>
       </c>
       <c r="DH2" s="4" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="3" spans="1:112" x14ac:dyDescent="0.2">
@@ -11441,6 +11463,12 @@
       <c r="DE3" t="s">
         <v>143</v>
       </c>
+      <c r="DG3" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH3" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="4" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -11620,6 +11648,12 @@
       <c r="DE4" t="s">
         <v>143</v>
       </c>
+      <c r="DG4" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH4" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="5" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -11799,6 +11833,12 @@
       <c r="DE5" t="s">
         <v>143</v>
       </c>
+      <c r="DG5" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH5" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="6" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -11978,6 +12018,12 @@
       <c r="DE6" t="s">
         <v>143</v>
       </c>
+      <c r="DG6" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH6" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="7" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -12157,6 +12203,12 @@
       <c r="DE7" t="s">
         <v>143</v>
       </c>
+      <c r="DG7" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH7" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="8" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -12333,6 +12385,12 @@
       <c r="DE8" t="s">
         <v>143</v>
       </c>
+      <c r="DG8" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH8" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="9" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -12509,6 +12567,12 @@
       <c r="DE9" t="s">
         <v>143</v>
       </c>
+      <c r="DG9" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH9" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="10" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -12685,6 +12749,12 @@
       <c r="DE10" t="s">
         <v>143</v>
       </c>
+      <c r="DG10" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH10" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="11" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -12861,6 +12931,12 @@
       <c r="DE11" t="s">
         <v>143</v>
       </c>
+      <c r="DG11" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH11" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="12" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -13040,6 +13116,12 @@
       <c r="DE12" t="s">
         <v>143</v>
       </c>
+      <c r="DG12" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH12" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="13" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -13219,6 +13301,12 @@
       <c r="DE13" t="s">
         <v>143</v>
       </c>
+      <c r="DG13" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH13" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="14" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -13395,6 +13483,12 @@
       <c r="DE14" t="s">
         <v>143</v>
       </c>
+      <c r="DG14" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH14" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="15" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -13571,6 +13665,12 @@
       <c r="DE15" t="s">
         <v>143</v>
       </c>
+      <c r="DG15" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH15" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="16" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -13750,8 +13850,14 @@
       <c r="DE16" t="s">
         <v>143</v>
       </c>
+      <c r="DG16" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH16" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="17" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>318</v>
       </c>
@@ -13929,8 +14035,14 @@
       <c r="DE17" t="s">
         <v>143</v>
       </c>
+      <c r="DG17" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH17" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="18" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>330</v>
       </c>
@@ -14105,8 +14217,14 @@
       <c r="DE18" t="s">
         <v>143</v>
       </c>
+      <c r="DG18" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH18" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="19" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>341</v>
       </c>
@@ -14281,8 +14399,14 @@
       <c r="DE19" t="s">
         <v>143</v>
       </c>
+      <c r="DG19" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH19" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="20" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>352</v>
       </c>
@@ -14457,8 +14581,14 @@
       <c r="DE20" t="s">
         <v>143</v>
       </c>
+      <c r="DG20" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH20" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="21" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>363</v>
       </c>
@@ -14633,8 +14763,14 @@
       <c r="DE21" t="s">
         <v>143</v>
       </c>
+      <c r="DG21" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH21" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="22" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>374</v>
       </c>
@@ -14812,8 +14948,14 @@
       <c r="DE22" t="s">
         <v>143</v>
       </c>
+      <c r="DG22" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH22" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="23" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>385</v>
       </c>
@@ -14988,8 +15130,14 @@
       <c r="DE23" t="s">
         <v>143</v>
       </c>
+      <c r="DG23" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH23" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="24" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>397</v>
       </c>
@@ -15167,8 +15315,14 @@
       <c r="DE24" t="s">
         <v>143</v>
       </c>
+      <c r="DG24" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH24" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="25" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>408</v>
       </c>
@@ -15346,8 +15500,14 @@
       <c r="DE25" t="s">
         <v>143</v>
       </c>
+      <c r="DG25" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH25" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="26" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>420</v>
       </c>
@@ -15525,8 +15685,14 @@
       <c r="DE26" t="s">
         <v>143</v>
       </c>
+      <c r="DG26" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH26" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="27" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>431</v>
       </c>
@@ -15704,8 +15870,14 @@
       <c r="DE27" t="s">
         <v>143</v>
       </c>
+      <c r="DG27" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH27" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="28" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>446</v>
       </c>
@@ -15883,8 +16055,14 @@
       <c r="DE28" t="s">
         <v>143</v>
       </c>
+      <c r="DG28" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH28" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="29" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>458</v>
       </c>
@@ -16065,8 +16243,14 @@
       <c r="DE29" t="s">
         <v>143</v>
       </c>
+      <c r="DG29" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH29" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="30" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>473</v>
       </c>
@@ -16244,8 +16428,14 @@
       <c r="DE30" t="s">
         <v>143</v>
       </c>
+      <c r="DG30" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH30" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="31" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>484</v>
       </c>
@@ -16423,8 +16613,14 @@
       <c r="DE31" t="s">
         <v>143</v>
       </c>
+      <c r="DG31" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH31" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
-    <row r="32" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>494</v>
       </c>
@@ -16598,6 +16794,12 @@
       </c>
       <c r="DE32" t="s">
         <v>143</v>
+      </c>
+      <c r="DG32" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH32" s="4" t="s">
+        <v>3281</v>
       </c>
     </row>
     <row r="33" spans="1:112" x14ac:dyDescent="0.2">
@@ -16778,6 +16980,12 @@
       <c r="DE33" t="s">
         <v>143</v>
       </c>
+      <c r="DG33" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH33" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="34" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -16958,10 +17166,10 @@
         <v>143</v>
       </c>
       <c r="DG34" s="4" t="s">
+        <v>3282</v>
+      </c>
+      <c r="DH34" s="4" t="s">
         <v>3277</v>
-      </c>
-      <c r="DH34" s="4" t="s">
-        <v>3278</v>
       </c>
     </row>
     <row r="35" spans="1:112" x14ac:dyDescent="0.2">
@@ -17145,6 +17353,12 @@
       <c r="DE35" t="s">
         <v>143</v>
       </c>
+      <c r="DG35" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH35" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="36" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -17321,6 +17535,12 @@
       <c r="DE36" t="s">
         <v>143</v>
       </c>
+      <c r="DG36" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH36" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="37" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -17497,6 +17717,12 @@
       <c r="DE37" t="s">
         <v>143</v>
       </c>
+      <c r="DG37" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH37" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="38" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -17673,6 +17899,12 @@
       <c r="DE38" t="s">
         <v>143</v>
       </c>
+      <c r="DG38" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH38" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="39" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -17852,6 +18084,12 @@
       <c r="DE39" t="s">
         <v>143</v>
       </c>
+      <c r="DG39" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH39" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="40" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -18032,10 +18270,10 @@
         <v>143</v>
       </c>
       <c r="DG40" s="4" t="s">
+        <v>3282</v>
+      </c>
+      <c r="DH40" s="4" t="s">
         <v>3277</v>
-      </c>
-      <c r="DH40" s="4" t="s">
-        <v>3278</v>
       </c>
     </row>
     <row r="41" spans="1:112" ht="17" x14ac:dyDescent="0.2">
@@ -18217,10 +18455,10 @@
         <v>143</v>
       </c>
       <c r="DG41" s="4" t="s">
+        <v>3282</v>
+      </c>
+      <c r="DH41" s="4" t="s">
         <v>3277</v>
-      </c>
-      <c r="DH41" s="4" t="s">
-        <v>3278</v>
       </c>
     </row>
     <row r="42" spans="1:112" ht="17" x14ac:dyDescent="0.2">
@@ -18408,7 +18646,7 @@
         <v>3276</v>
       </c>
       <c r="DH42" s="4" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="43" spans="1:112" ht="17" x14ac:dyDescent="0.2">
@@ -18590,10 +18828,10 @@
         <v>143</v>
       </c>
       <c r="DG43" s="4" t="s">
-        <v>3279</v>
+        <v>3278</v>
       </c>
       <c r="DH43" s="4" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="44" spans="1:112" ht="17" x14ac:dyDescent="0.2">
@@ -18778,10 +19016,10 @@
         <v>143</v>
       </c>
       <c r="DG44" s="4" t="s">
+        <v>3282</v>
+      </c>
+      <c r="DH44" s="4" t="s">
         <v>3277</v>
-      </c>
-      <c r="DH44" s="4" t="s">
-        <v>3278</v>
       </c>
     </row>
     <row r="45" spans="1:112" ht="17" x14ac:dyDescent="0.2">
@@ -18966,10 +19204,10 @@
         <v>143</v>
       </c>
       <c r="DG45" s="4" t="s">
-        <v>3280</v>
+        <v>3279</v>
       </c>
       <c r="DH45" s="4" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="46" spans="1:112" x14ac:dyDescent="0.2">
@@ -19150,6 +19388,12 @@
       <c r="DE46" t="s">
         <v>143</v>
       </c>
+      <c r="DG46" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH46" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="47" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -19329,6 +19573,12 @@
       <c r="DE47" t="s">
         <v>143</v>
       </c>
+      <c r="DG47" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH47" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="48" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -19508,6 +19758,12 @@
       <c r="DE48" t="s">
         <v>143</v>
       </c>
+      <c r="DG48" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH48" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="49" spans="1:112" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -19688,10 +19944,10 @@
         <v>143</v>
       </c>
       <c r="DG49" s="4" t="s">
+        <v>3282</v>
+      </c>
+      <c r="DH49" s="4" t="s">
         <v>3277</v>
-      </c>
-      <c r="DH49" s="4" t="s">
-        <v>3278</v>
       </c>
     </row>
     <row r="50" spans="1:112" x14ac:dyDescent="0.2">
@@ -19872,6 +20128,12 @@
       <c r="DE50" t="s">
         <v>143</v>
       </c>
+      <c r="DG50" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH50" s="4" t="s">
+        <v>3281</v>
+      </c>
     </row>
     <row r="51" spans="1:112" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -20058,10 +20320,10 @@
         <v>143</v>
       </c>
       <c r="DG51" s="4" t="s">
-        <v>3280</v>
+        <v>3279</v>
       </c>
       <c r="DH51" s="4" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="52" spans="1:112" ht="17" x14ac:dyDescent="0.2">
@@ -20243,10 +20505,10 @@
         <v>143</v>
       </c>
       <c r="DG52" s="4" t="s">
+        <v>3282</v>
+      </c>
+      <c r="DH52" s="4" t="s">
         <v>3277</v>
-      </c>
-      <c r="DH52" s="4" t="s">
-        <v>3278</v>
       </c>
     </row>
     <row r="53" spans="1:112" ht="17" x14ac:dyDescent="0.2">
@@ -20431,7 +20693,7 @@
         <v>3276</v>
       </c>
       <c r="DH53" s="5" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="54" spans="1:112" x14ac:dyDescent="0.2">
@@ -20611,6 +20873,12 @@
       </c>
       <c r="DE54" t="s">
         <v>143</v>
+      </c>
+      <c r="DG54" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="DH54" s="4" t="s">
+        <v>3281</v>
       </c>
     </row>
     <row r="55" spans="1:112" x14ac:dyDescent="0.2">
@@ -59682,4 +59950,74 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B7DB46-59E0-6F40-9236-B0C9B0D61973}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>3275</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>3281</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>3282</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>3283</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>3286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>3287</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
LOV for charred decayClass
</commit_message>
<xml_diff>
--- a/cdw_tallyAnalysis/D17/D17-SOAP-2023_cdw_tally_prod_child.xlsx
+++ b/cdw_tallyAnalysis/D17/D17-SOAP-2023_cdw_tally_prod_child.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmeier/Documents/gitRepositories/neon-plant-sampling/cdw_tallyAnalysis/D17/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2168AD-1D66-4344-994D-FEDDDEEF2CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CE2EE1-703C-2240-B7DE-788E081A79E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12500" yWindow="500" windowWidth="37340" windowHeight="28300" activeTab="1" xr2:uid="{75547C8C-A164-894F-9105-1D1F1743C90B}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11929" uniqueCount="3288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11933" uniqueCount="3292">
   <si>
     <t>_child_record_id</t>
   </si>
@@ -9886,6 +9886,18 @@
   </si>
   <si>
     <t>96-100</t>
+  </si>
+  <si>
+    <t>decayClass</t>
+  </si>
+  <si>
+    <t>charred - sound</t>
+  </si>
+  <si>
+    <t>charred - moderate</t>
+  </si>
+  <si>
+    <t>charred - advanced</t>
   </si>
 </sst>
 </file>
@@ -59954,65 +59966,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B7DB46-59E0-6F40-9236-B0C9B0D61973}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3275</v>
       </c>
       <c r="B1" t="s">
         <v>3274</v>
       </c>
+      <c r="C1" t="s">
+        <v>3288</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3281</v>
       </c>
       <c r="B2" t="s">
         <v>3281</v>
       </c>
+      <c r="C2" t="s">
+        <v>3289</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3282</v>
       </c>
       <c r="B3" t="s">
         <v>3277</v>
       </c>
+      <c r="C3" t="s">
+        <v>3290</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3283</v>
       </c>
       <c r="B4" t="s">
         <v>3280</v>
       </c>
+      <c r="C4" t="s">
+        <v>3291</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3284</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>3285</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>3286</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3287</v>
       </c>

</xml_diff>